<commit_message>
Updated DH params spreasheet
</commit_message>
<xml_diff>
--- a/DH_Parameters.xlsx
+++ b/DH_Parameters.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="995" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Spine" sheetId="1" state="visible" r:id="rId2"/>
@@ -103,6 +103,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-s</t>
     </r>
@@ -112,6 +113,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(</t>
     </r>
@@ -120,6 +122,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">th_1</t>
     </r>
@@ -129,6 +132,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
@@ -225,11 +229,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -248,6 +253,12 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -351,7 +362,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -433,6 +444,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -472,14 +487,14 @@
   <dimension ref="B2:L23"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="L10" activeCellId="0" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="7" min="1" style="0" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="12" min="8" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="7" min="1" style="0" width="11.8061224489796"/>
+    <col collapsed="false" hidden="false" max="12" min="8" style="0" width="18.5561224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="9.31632653061224"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -550,7 +565,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="13" t="n">
-        <v>0</v>
+        <v>-16.975</v>
       </c>
       <c r="E4" s="13" t="n">
         <v>0</v>
@@ -632,8 +647,8 @@
       <c r="K10" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="L10" s="6" t="n">
-        <v>0</v>
+      <c r="L10" s="21" t="n">
+        <v>-16.975</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -843,9 +858,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="7" min="1" style="0" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="12" min="8" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="7" min="1" style="0" width="11.8061224489796"/>
+    <col collapsed="false" hidden="false" max="12" min="8" style="0" width="18.5561224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="9.31632653061224"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1006,13 +1021,13 @@
       <c r="B8" s="10" t="n">
         <v>5</v>
       </c>
-      <c r="C8" s="21" t="n">
+      <c r="C8" s="22" t="n">
         <v>-90</v>
       </c>
-      <c r="D8" s="21" t="n">
+      <c r="D8" s="22" t="n">
         <v>45.032</v>
       </c>
-      <c r="E8" s="21" t="n">
+      <c r="E8" s="22" t="n">
         <v>0</v>
       </c>
       <c r="F8" s="12" t="s">
@@ -1020,19 +1035,19 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="23" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" s="23" t="n">
+      <c r="C9" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="24" t="n">
         <v>33.596</v>
       </c>
-      <c r="E9" s="23" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" s="24" t="n">
+      <c r="E9" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="25" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1439,7 +1454,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>